<commit_message>
change qty rules for Rust and MtB Products
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -85,9 +85,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -115,24 +115,48 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,32 +168,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,9 +199,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,16 +213,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,37 +245,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,49 +267,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,133 +429,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,24 +458,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -490,6 +472,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,21 +530,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -558,153 +540,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
add create product into erp system
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowHeight="17850"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -32,34 +32,55 @@
     <t>Product_id</t>
   </si>
   <si>
+    <t>Vintage1</t>
+  </si>
+  <si>
+    <t>Vintage2</t>
+  </si>
+  <si>
+    <t>Product_code1</t>
+  </si>
+  <si>
+    <t>Product_code2</t>
+  </si>
+  <si>
+    <t>Quantity1</t>
+  </si>
+  <si>
+    <t>Quantity2</t>
+  </si>
+  <si>
+    <t>This is testing for adding MtB product into ERP system</t>
+  </si>
+  <si>
+    <t>Winery</t>
+  </si>
+  <si>
+    <t>MtB Winery - Garage Cellar</t>
+  </si>
+  <si>
+    <t>Modest Wines - Gruner</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Modest Wines - By Jove 2019</t>
+  </si>
+  <si>
+    <t>61419-19</t>
+  </si>
+  <si>
+    <t>61419-20</t>
+  </si>
+  <si>
+    <t>MtB Winery - Floor</t>
+  </si>
+  <si>
     <t>Product_code</t>
   </si>
   <si>
     <t>Quantity</t>
-  </si>
-  <si>
-    <t>This is testing for adding MtB product into ERP system</t>
-  </si>
-  <si>
-    <t>Winery</t>
-  </si>
-  <si>
-    <t>MtB Winery - Garage Cellar</t>
-  </si>
-  <si>
-    <t>Modest Wines - By Jove 2019</t>
-  </si>
-  <si>
-    <t>61419-19</t>
-  </si>
-  <si>
-    <t>Modest Wines - By Jove 2020</t>
-  </si>
-  <si>
-    <t>61419-20</t>
-  </si>
-  <si>
-    <t>MtB Winery - Floor</t>
   </si>
   <si>
     <t>This is testing for adding Rust product into ERP system</t>
@@ -85,10 +106,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -114,13 +135,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,25 +143,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,40 +181,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -213,9 +221,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,27 +244,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -252,7 +273,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,19 +288,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,127 +426,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,31 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,6 +479,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,65 +571,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -563,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -572,139 +593,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1040,23 +1061,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="32.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="22.4444444444444" style="3" customWidth="1"/>
+    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="22.447619047619" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.3333333333333" style="3" customWidth="1"/>
-    <col min="4" max="5" width="29.4444444444444" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.1111111111111" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.3333333333333" style="3" customWidth="1"/>
+    <col min="4" max="7" width="29.447619047619" style="3" customWidth="1"/>
+    <col min="8" max="9" width="20.1142857142857" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.3333333333333" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:7">
+    <row r="1" ht="15.75" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,96 +1099,121 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" ht="15.6" spans="1:7">
+    <row r="2" ht="15.75" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>61419</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>78235</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3">
+        <v>78235</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3">
         <v>11</v>
       </c>
-      <c r="G2" s="2">
-        <v>18</v>
+      <c r="K2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:7">
+    <row r="3" ht="15.75" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>61419</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
+      <c r="F3" s="2">
+        <v>2019</v>
       </c>
       <c r="G3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2">
         <v>188</v>
       </c>
     </row>
-    <row r="4" ht="15.6" spans="1:7">
+    <row r="4" ht="15.75" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>61420</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>61419</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2019</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="15.6" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2">
-        <v>61421</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="3">
         <v>147</v>
       </c>
     </row>
@@ -1182,21 +1228,21 @@
   <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="41.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="41.447619047619" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.4444444444444" customWidth="1"/>
-    <col min="4" max="5" width="27.1111111111111" customWidth="1"/>
-    <col min="6" max="6" width="21.8888888888889" customWidth="1"/>
-    <col min="7" max="7" width="16.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="22.447619047619" customWidth="1"/>
+    <col min="4" max="5" width="27.1142857142857" customWidth="1"/>
+    <col min="6" max="6" width="21.8857142857143" customWidth="1"/>
+    <col min="7" max="7" width="16.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:7">
+    <row r="1" ht="15.75" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,53 +1259,53 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:7">
+    <row r="2" ht="15.75" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2">
         <v>150461</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:7">
+    <row r="3" ht="15.75" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2">
         <v>150461</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2">
         <v>246</v>

</xml_diff>

<commit_message>
add mobile emulator test
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Description</t>
   </si>
@@ -59,19 +59,22 @@
     <t>MtB Winery - Garage Cellar</t>
   </si>
   <si>
+    <t>Modest Wines - By Jove 2019</t>
+  </si>
+  <si>
+    <t>61419-19</t>
+  </si>
+  <si>
+    <t>61419-20</t>
+  </si>
+  <si>
+    <t>//This is testing for adding MtB product into ERP system</t>
+  </si>
+  <si>
     <t>Modest Wines - Gruner</t>
   </si>
   <si>
     <t>NULL</t>
-  </si>
-  <si>
-    <t>Modest Wines - By Jove 2019</t>
-  </si>
-  <si>
-    <t>61419-19</t>
-  </si>
-  <si>
-    <t>61419-20</t>
   </si>
   <si>
     <t>MtB Winery - Floor</t>
@@ -106,10 +109,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -135,16 +138,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,48 +229,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,71 +261,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -294,19 +297,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +399,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,42 +441,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -378,55 +453,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,37 +471,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,11 +487,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,21 +533,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -556,6 +557,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -570,15 +582,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -593,139 +596,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1061,13 +1064,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="22.447619047619" style="3" customWidth="1"/>
@@ -1122,34 +1125,34 @@
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3">
-        <v>78235</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2">
+        <v>61419</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3">
-        <v>78235</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="3">
-        <v>11</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2">
+        <v>188</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -1157,43 +1160,43 @@
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>61419</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2020</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2">
-        <v>18</v>
-      </c>
-      <c r="K3" s="2">
-        <v>188</v>
+      <c r="E3" s="3">
+        <v>78235</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3">
+        <v>78235</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>61419</v>
@@ -1205,15 +1208,50 @@
         <v>2020</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
+        <v>61419</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="3">
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="3">
         <v>147</v>
       </c>
     </row>
@@ -1259,30 +1297,30 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2">
         <v>150461</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -1290,22 +1328,22 @@
     </row>
     <row r="3" ht="15.75" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2">
         <v>150461</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2">
         <v>246</v>

</xml_diff>

<commit_message>
add barcode into excel test data
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -50,6 +50,12 @@
     <t>Quantity2</t>
   </si>
   <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>SCC</t>
+  </si>
+  <si>
     <t>This is testing for adding MtB product into ERP system</t>
   </si>
   <si>
@@ -59,6 +65,18 @@
     <t>MtB Winery - Garage Cellar</t>
   </si>
   <si>
+    <t>Modest Wines - Gruner</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>812289292694</t>
+  </si>
+  <si>
+    <t>10812288192695</t>
+  </si>
+  <si>
     <t>Modest Wines - By Jove 2019</t>
   </si>
   <si>
@@ -68,13 +86,22 @@
     <t>61419-20</t>
   </si>
   <si>
-    <t>Modest Wines - Gruner</t>
-  </si>
-  <si>
-    <t>NULL</t>
+    <t>812289192693</t>
+  </si>
+  <si>
+    <t>10812289192690</t>
   </si>
   <si>
     <t>MtB Winery - Floor</t>
+  </si>
+  <si>
+    <t>Mt. Boucherie - Bubbles</t>
+  </si>
+  <si>
+    <t>812289165109</t>
+  </si>
+  <si>
+    <t>10122891651097</t>
   </si>
   <si>
     <t>Product_code</t>
@@ -106,12 +133,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +162,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -144,6 +200,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -151,7 +214,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,45 +282,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -214,9 +292,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -227,53 +312,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,192 +329,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -482,17 +523,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="medium">
+        <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,7 +542,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,8 +565,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,17 +601,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,11 +621,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,7 +640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -602,134 +658,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -742,6 +798,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,10 +1136,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1072,12 +1147,18 @@
     <col min="1" max="1" width="42.1388888888889" customWidth="1"/>
     <col min="2" max="2" width="22.4444444444444" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.3333333333333" style="3" customWidth="1"/>
-    <col min="4" max="7" width="29.4444444444444" style="3" customWidth="1"/>
-    <col min="8" max="9" width="20.1111111111111" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.3333333333333" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.4444444444444" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.7777777777778" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.55555555555556" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.1111111111111" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.6666666666667" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.77777777777778" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="16.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:11">
+    <row r="1" ht="15.6" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,89 +1192,107 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" ht="15.6" spans="1:11">
+    <row r="2" ht="15.6" spans="1:13">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4">
+        <v>78235</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4">
+        <v>78235</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="15.6" spans="1:13">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
         <v>61419</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>2019</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <v>2020</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="6">
         <v>18</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K3" s="6">
         <v>188</v>
       </c>
+      <c r="L3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" ht="15.6" spans="1:11">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="4" ht="16.35" spans="1:13">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3">
-        <v>78235</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3">
-        <v>78235</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="3">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" ht="15.6" spans="1:11">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2">
         <v>61419</v>
@@ -1205,51 +1304,63 @@
         <v>2020</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2">
-        <v>188</v>
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="6">
+        <v>147</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" ht="15.6" spans="1:11">
+    <row r="5" ht="15.6" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2">
-        <v>61419</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2020</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="4">
+        <v>160920</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4">
+        <v>160920</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="3">
-        <v>147</v>
+        <v>17</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1294,30 +1405,30 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2">
         <v>150461</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -1325,22 +1436,22 @@
     </row>
     <row r="3" ht="15.6" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2">
         <v>150461</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2">
         <v>246</v>

</xml_diff>

<commit_message>
add vintage quantity method
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -65,6 +65,21 @@
     <t>MtB Winery - Garage Cellar</t>
   </si>
   <si>
+    <t>Modest Wines - By Jove 2019</t>
+  </si>
+  <si>
+    <t>61419-19</t>
+  </si>
+  <si>
+    <t>61419-20</t>
+  </si>
+  <si>
+    <t>812289192693</t>
+  </si>
+  <si>
+    <t>10812289192690</t>
+  </si>
+  <si>
     <t>Modest Wines - Gruner</t>
   </si>
   <si>
@@ -75,21 +90,6 @@
   </si>
   <si>
     <t>10812288192695</t>
-  </si>
-  <si>
-    <t>Modest Wines - By Jove 2019</t>
-  </si>
-  <si>
-    <t>61419-19</t>
-  </si>
-  <si>
-    <t>61419-20</t>
-  </si>
-  <si>
-    <t>812289192693</t>
-  </si>
-  <si>
-    <t>10812289192690</t>
   </si>
   <si>
     <t>MtB Winery - Floor</t>
@@ -133,10 +133,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -177,6 +177,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -184,75 +252,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,31 +283,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -299,22 +314,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -329,187 +329,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,11 +538,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,8 +571,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,6 +588,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,8 +619,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,27 +635,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -658,134 +658,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -796,9 +796,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1138,8 +1135,8 @@
   <sheetPr/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1192,10 +1189,10 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1212,32 +1209,32 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4">
-        <v>78235</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>61419</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="4">
-        <v>78235</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="J2" s="5">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5">
+        <v>188</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>19</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="15.6" spans="1:13">
@@ -1251,33 +1248,33 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2">
-        <v>61419</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2020</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>78235</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2">
+        <v>78235</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="6">
-        <v>18</v>
-      </c>
-      <c r="K3" s="6">
-        <v>188</v>
-      </c>
-      <c r="L3" s="10" t="s">
+      <c r="J3" s="5">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1292,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>61419</v>
@@ -1304,22 +1301,22 @@
         <v>2020</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>147</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>24</v>
+      <c r="L4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" ht="15.6" spans="1:13">
@@ -1335,31 +1332,31 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>160920</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="4">
+        <v>22</v>
+      </c>
+      <c r="H5" s="2">
         <v>160920</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="4">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2">
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="11" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add select source location
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" activeTab="2"/>
+    <workbookView windowHeight="17850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Agency Warehouse: Internal Transfers</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Garage Cellar</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Floor</t>
   </si>
 </sst>
 </file>
@@ -183,12 +189,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,9 +226,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,6 +257,83 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,41 +345,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,38 +360,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,20 +374,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,13 +381,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -379,187 +391,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,21 +596,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,11 +639,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,15 +689,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -690,152 +702,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -857,7 +869,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -865,7 +880,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1189,13 +1204,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="22.447619047619" style="1" customWidth="1"/>
@@ -1334,10 +1349,10 @@
       <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1399,10 +1414,10 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1464,10 +1479,10 @@
       <c r="S4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1529,30 +1544,12 @@
       <c r="S5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" spans="1:7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" ht="15.75" spans="1:7">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1660,10 +1657,10 @@
       <c r="K2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1701,10 +1698,10 @@
       <c r="K3" s="5">
         <v>188</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1742,10 +1739,10 @@
       <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1783,10 +1780,10 @@
       <c r="K5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1819,8 +1816,8 @@
   <sheetPr/>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1928,7 +1925,7 @@
       <c r="F2" s="3">
         <v>2019</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>42</v>
       </c>
       <c r="H2" s="3">
@@ -1943,7 +1940,7 @@
       <c r="K2" s="3">
         <v>2013</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>43</v>
       </c>
       <c r="M2" s="3">
@@ -1967,10 +1964,10 @@
       <c r="S2" s="3">
         <v>50</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="14" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2032,10 +2029,10 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="U3" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2050,14 +2047,14 @@
   <sheetPr/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="22.447619047619" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="12.4285714285714" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.3333333333333" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.447619047619" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.7809523809524" style="1" customWidth="1"/>
@@ -2123,7 +2120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:14">
+    <row r="2" ht="15.75" spans="1:16">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -2157,14 +2154,20 @@
       <c r="K2" s="5">
         <v>188</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N2" t="s">
         <v>52</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:13">
@@ -2201,10 +2204,10 @@
       <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2242,10 +2245,10 @@
       <c r="K4" s="5">
         <v>147</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2283,10 +2286,10 @@
       <c r="K5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="13" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add deliver address method
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -166,6 +166,9 @@
     <t>10812289292581</t>
   </si>
   <si>
+    <t>Deliver_address</t>
+  </si>
+  <si>
     <t>Operation_type</t>
   </si>
   <si>
@@ -185,6 +188,15 @@
   </si>
   <si>
     <t>Modest Wines - By Jove 2019 (T3394)</t>
+  </si>
+  <si>
+    <t>Counter Sale - MB</t>
+  </si>
+  <si>
+    <t>Sonny International: Delivery Orders</t>
+  </si>
+  <si>
+    <t>SI/Stock</t>
   </si>
   <si>
     <t>Agency Warehouse: Internal Transfers</t>
@@ -253,48 +265,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -303,6 +273,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -327,6 +326,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -335,6 +341,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -360,7 +373,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,29 +408,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -406,187 +418,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,6 +642,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -654,37 +681,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,12 +713,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -735,134 +747,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -872,22 +884,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -912,9 +918,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1323,270 +1326,270 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:21">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>78235</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="12">
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="10">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="16" t="s">
+      <c r="N2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:21">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>61419</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>2019</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>2020</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="12">
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="10">
         <v>18</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="10">
         <v>188</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="16" t="s">
+      <c r="O3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:21">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>61419</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>2019</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2020</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="12">
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="10">
         <v>147</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>0</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="16" t="s">
+      <c r="O4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:21">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>160920</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="3">
         <v>500</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T5" s="17" t="s">
+      <c r="N5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1655,194 +1658,194 @@
       <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>78235</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3">
         <v>78235</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="12">
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="10">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="16" t="s">
+      <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:13">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>61419</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>2019</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>2020</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="10">
         <v>18</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="10">
         <v>188</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:13">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>61419</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>2019</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2020</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>147</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:13">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>160920</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3">
         <v>160920</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3">
         <v>500</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="17" t="s">
+      <c r="K5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:7">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" ht="15.75" spans="1:7">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1938,140 +1941,140 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:21">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>150461</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>2019</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>2022</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>2018</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>2021</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>2013</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <v>1000</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>2000</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>300</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>10</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>1</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="3">
         <v>246</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="3">
         <v>50</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="U2" s="17" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:21">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>150461</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>2020</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>2021</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>246</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="19" t="s">
+      <c r="O3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="U3" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2084,10 +2087,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -2098,14 +2101,14 @@
     <col min="4" max="4" width="9.55238095238095" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.33333333333333" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="16.8857142857143" customWidth="1"/>
-    <col min="8" max="8" width="34.2857142857143" customWidth="1"/>
-    <col min="9" max="9" width="15.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="7" max="8" width="16.8857142857143" customWidth="1"/>
+    <col min="9" max="9" width="34.2857142857143" customWidth="1"/>
+    <col min="10" max="10" width="15.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:12">
+    <row r="1" ht="15.75" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2121,149 +2124,161 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" spans="1:12">
-      <c r="A2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" ht="15.75" spans="1:10">
+      <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3">
         <v>61419</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>2019</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>2020</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="6">
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:13">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3">
+        <v>78235</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="3">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>59</v>
+      <c r="M3" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:12">
-      <c r="A3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4">
-        <v>78235</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+    <row r="4" ht="16.5" spans="1:13">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3">
+        <v>61419</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
-    <row r="4" ht="16.5" spans="1:12">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4">
-        <v>61419</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2019</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" ht="15.75" spans="1:12">
-      <c r="A5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" ht="15.75" spans="1:13">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>160920</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="19" t="s">
         <v>34</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add transfer delivery order and internal transfer
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -8,16 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
-    <sheet name="test_add_MtB (2)" sheetId="6" r:id="rId2"/>
-    <sheet name="test_add_Rust" sheetId="4" r:id="rId3"/>
-    <sheet name="test_internal_transfer" sheetId="5" r:id="rId4"/>
+    <sheet name="test_add_Rust" sheetId="4" r:id="rId2"/>
+    <sheet name="test_internal_transfer" sheetId="5" r:id="rId3"/>
+    <sheet name="test_transfer_delivery_order" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -124,18 +124,6 @@
     <t>10122891651097</t>
   </si>
   <si>
-    <t>Product_code1</t>
-  </si>
-  <si>
-    <t>Product_code2</t>
-  </si>
-  <si>
-    <t>61419-19</t>
-  </si>
-  <si>
-    <t>61419-20</t>
-  </si>
-  <si>
     <t>This is testing for adding Rust product into ERP system</t>
   </si>
   <si>
@@ -166,6 +154,12 @@
     <t>10812289292581</t>
   </si>
   <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
     <t>Deliver_address</t>
   </si>
   <si>
@@ -178,18 +172,42 @@
     <t>Destination_Location</t>
   </si>
   <si>
-    <t>Demand</t>
-  </si>
-  <si>
-    <t>Unit_of_Measure</t>
+    <t>Demand1</t>
+  </si>
+  <si>
+    <t>Demand2</t>
+  </si>
+  <si>
+    <t>Unit_of_Measure1</t>
+  </si>
+  <si>
+    <t>Unit_of_Measure2</t>
   </si>
   <si>
     <t>This is testing with internal transfer for  MtB product</t>
   </si>
   <si>
+    <t>Agency Warehouse: Internal Transfers</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Garage Cellar</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Floor</t>
+  </si>
+  <si>
+    <t>Case12</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Delivery Orders" for  MtB product</t>
+  </si>
+  <si>
     <t>Modest Wines - By Jove 2019 (T3394)</t>
   </si>
   <si>
+    <t>Modest Wines - By Jove 2019 (T4156)</t>
+  </si>
+  <si>
     <t>Counter Sale - MB</t>
   </si>
   <si>
@@ -197,18 +215,6 @@
   </si>
   <si>
     <t>SI/Stock</t>
-  </si>
-  <si>
-    <t>Agency Warehouse: Internal Transfers</t>
-  </si>
-  <si>
-    <t>WH/MtB Winery - Garage Cellar</t>
-  </si>
-  <si>
-    <t>WH/MtB Winery - Floor</t>
-  </si>
-  <si>
-    <t>Case12</t>
   </si>
 </sst>
 </file>
@@ -216,10 +222,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -240,12 +246,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -265,6 +265,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -273,8 +293,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,112 +401,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -418,12 +424,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -436,169 +598,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,36 +629,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,11 +657,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -729,82 +735,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -813,68 +819,68 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -887,22 +893,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -911,21 +908,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1249,7 +1240,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1326,10 +1317,10 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1370,7 +1361,7 @@
       <c r="L2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="7">
         <v>11</v>
       </c>
       <c r="N2" s="3" t="s">
@@ -1391,10 +1382,10 @@
       <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1435,10 +1426,10 @@
       <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>18</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="7">
         <v>188</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -1456,10 +1447,10 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1500,7 +1491,7 @@
       <c r="L4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="7">
         <v>147</v>
       </c>
       <c r="N4" s="3">
@@ -1521,10 +1512,10 @@
       <c r="S4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="14" t="s">
+      <c r="U4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1586,10 +1577,10 @@
       <c r="S5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="16" t="s">
+      <c r="U5" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1602,264 +1593,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="22.447619047619" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.4285714285714" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.447619047619" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7809523809524" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5714285714286" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="16.8857142857143" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.75" spans="1:13">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:13">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3">
-        <v>78235</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3">
-        <v>78235</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="10">
-        <v>11</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:13">
-      <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="3">
-        <v>61419</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2019</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2020</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="10">
-        <v>18</v>
-      </c>
-      <c r="K3" s="10">
-        <v>188</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" ht="16.5" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3">
-        <v>61419</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2020</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="10">
-        <v>147</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:13">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3">
-        <v>160920</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3">
-        <v>160920</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3">
-        <v>500</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" ht="15.75" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1941,25 +1678,25 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:21">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3">
         <v>150461</v>
@@ -1967,8 +1704,8 @@
       <c r="F2" s="3">
         <v>2019</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>42</v>
+      <c r="G2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="H2" s="3">
         <v>2022</v>
@@ -1982,8 +1719,8 @@
       <c r="K2" s="3">
         <v>2013</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>43</v>
+      <c r="L2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="M2" s="3">
         <v>1000</v>
@@ -2006,25 +1743,25 @@
       <c r="S2" s="3">
         <v>50</v>
       </c>
-      <c r="T2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>45</v>
+      <c r="T2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:21">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3">
         <v>150461</v>
@@ -2071,11 +1808,107 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="29.447619047619" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7809523809524" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.8857142857143" customWidth="1"/>
+    <col min="5" max="5" width="34.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="15.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3">
+        <v>78235</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2087,36 +1920,37 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="29.447619047619" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7809523809524" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.55238095238095" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="16.8857142857143" customWidth="1"/>
-    <col min="9" max="9" width="34.2857142857143" customWidth="1"/>
-    <col min="10" max="10" width="15.5714285714286" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="15.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="20.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="19.2857142857143" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="35.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:13">
+    <row r="1" ht="15.75" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -2125,160 +1959,64 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row r="2" ht="15.75" spans="1:10">
+    <row r="2" s="1" customFormat="1" ht="15.75" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="3">
-        <v>61419</v>
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="3">
         <v>2019</v>
       </c>
       <c r="E2" s="3">
-        <v>2020</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>30</v>
+        <v>2019</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:13">
-      <c r="A3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3">
-        <v>78235</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="3">
-        <v>12</v>
-      </c>
-      <c r="M3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" ht="16.5" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3">
-        <v>61419</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2020</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" ht="15.75" spans="1:13">
-      <c r="A5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3">
-        <v>160920</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update internal transfer test
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -154,6 +154,48 @@
     <t>10812289292581</t>
   </si>
   <si>
+    <t>Product_code</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Unit_of_Measure1</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Operation_type</t>
+  </si>
+  <si>
+    <t>Source_location</t>
+  </si>
+  <si>
+    <t>Destination_location</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Internal Transfer" for  MtB product</t>
+  </si>
+  <si>
+    <t>Summit Double Magnum 3L</t>
+  </si>
+  <si>
+    <t>140743-19</t>
+  </si>
+  <si>
+    <t>Craig Demo</t>
+  </si>
+  <si>
+    <t>Sonny International: Internal Transfers</t>
+  </si>
+  <si>
+    <t>WH/Mt. Boucherie Winery</t>
+  </si>
+  <si>
+    <t>SI/Stock</t>
+  </si>
+  <si>
     <t>Product1</t>
   </si>
   <si>
@@ -166,47 +208,20 @@
     <t>Demand2</t>
   </si>
   <si>
-    <t>Unit_of_Measure1</t>
-  </si>
-  <si>
     <t>Unit_of_Measure2</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Operation_type</t>
-  </si>
-  <si>
-    <t>Source_location</t>
-  </si>
-  <si>
-    <t>Destination_location</t>
+    <t>Deliver_address</t>
+  </si>
+  <si>
+    <t>Source_Location</t>
   </si>
   <si>
     <t>This is testing "Transfer" with "Delivery Orders" for  MtB product</t>
-  </si>
-  <si>
-    <t>Summit Double Magnum 3L</t>
   </si>
   <si>
     <t xml:space="preserve">Rose 750ml
 </t>
-  </si>
-  <si>
-    <t>Sonny International: Internal Transfers</t>
-  </si>
-  <si>
-    <t>WH/Mt. Boucherie Winery</t>
-  </si>
-  <si>
-    <t>SI/Stock</t>
-  </si>
-  <si>
-    <t>Deliver_address</t>
-  </si>
-  <si>
-    <t>Source_Location</t>
   </si>
   <si>
     <t>Counter Sale - MB</t>
@@ -221,11 +236,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,12 +264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.75"/>
-      <color rgb="FF66598F"/>
-      <name val="Helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +278,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,24 +354,54 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,103 +415,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -422,181 +431,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,13 +640,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,22 +689,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,22 +698,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,9 +729,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,152 +742,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,13 +900,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -906,12 +912,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1237,27 +1243,27 @@
   <sheetPr/>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="22.447619047619" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.4285714285714" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.447619047619" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7809523809524" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5714285714286" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="22.4444444444444" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.4259259259259" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.4444444444444" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7777777777778" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5740740740741" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1142857142857" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1111111111111" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.287037037037" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="16.8857142857143" customWidth="1"/>
+    <col min="13" max="13" width="16.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.6" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1315,14 +1321,14 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:21">
+    <row r="2" ht="15.6" spans="1:21">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1359,7 +1365,7 @@
       <c r="L2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <v>11</v>
       </c>
       <c r="N2" s="3" t="s">
@@ -1380,14 +1386,14 @@
       <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:21">
+    <row r="3" ht="15.6" spans="1:21">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1424,10 +1430,10 @@
       <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>18</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="6">
         <v>188</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -1445,14 +1451,14 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" ht="16.5" spans="1:21">
+    <row r="4" ht="16.35" spans="1:21">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1489,7 +1495,7 @@
       <c r="L4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>147</v>
       </c>
       <c r="N4" s="3">
@@ -1510,14 +1516,14 @@
       <c r="S4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="U4" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:21">
+    <row r="5" ht="15.6" spans="1:21">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1575,10 +1581,10 @@
       <c r="S5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1594,31 +1600,31 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="41.447619047619" customWidth="1"/>
+    <col min="1" max="1" width="41.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.447619047619" customWidth="1"/>
-    <col min="4" max="4" width="27.1142857142857" customWidth="1"/>
-    <col min="5" max="5" width="12.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="9.42857142857143" customWidth="1"/>
-    <col min="7" max="7" width="9.71428571428571" customWidth="1"/>
-    <col min="8" max="8" width="9.57142857142857" customWidth="1"/>
+    <col min="3" max="3" width="22.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="27.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="12.1388888888889" customWidth="1"/>
+    <col min="6" max="6" width="9.42592592592593" customWidth="1"/>
+    <col min="7" max="7" width="9.71296296296296" customWidth="1"/>
+    <col min="8" max="8" width="9.57407407407407" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="9.71428571428571" customWidth="1"/>
-    <col min="12" max="12" width="9.57142857142857" customWidth="1"/>
-    <col min="13" max="13" width="11.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="11.1428571428571" customWidth="1"/>
-    <col min="15" max="15" width="10.8571428571429" customWidth="1"/>
-    <col min="16" max="16" width="11.2857142857143" customWidth="1"/>
-    <col min="19" max="19" width="11.2857142857143" customWidth="1"/>
+    <col min="10" max="10" width="10.287037037037" customWidth="1"/>
+    <col min="11" max="11" width="9.71296296296296" customWidth="1"/>
+    <col min="12" max="12" width="9.57407407407407" customWidth="1"/>
+    <col min="13" max="13" width="11.8611111111111" customWidth="1"/>
+    <col min="14" max="14" width="11.1388888888889" customWidth="1"/>
+    <col min="15" max="15" width="10.8611111111111" customWidth="1"/>
+    <col min="16" max="16" width="11.287037037037" customWidth="1"/>
+    <col min="19" max="19" width="11.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.6" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1676,14 +1682,14 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:21">
+    <row r="2" ht="15.6" spans="1:21">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1702,7 +1708,7 @@
       <c r="F2" s="3">
         <v>2019</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="3">
@@ -1717,7 +1723,7 @@
       <c r="K2" s="3">
         <v>2013</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M2" s="3">
@@ -1741,14 +1747,14 @@
       <c r="S2" s="3">
         <v>50</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:21">
+    <row r="3" ht="15.6" spans="1:21">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -1806,10 +1812,10 @@
       <c r="S3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1822,112 +1828,86 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="22.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="29.447619047619" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5714285714286" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="15.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="15.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="11.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="16.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="11.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="18.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
-    <col min="13" max="13" width="22.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="29.4444444444444" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5740740740741" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.287037037037" customWidth="1"/>
+    <col min="5" max="5" width="16.8611111111111" customWidth="1"/>
+    <col min="6" max="6" width="10.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="18.4259259259259" customWidth="1"/>
+    <col min="8" max="8" width="19.712962962963" customWidth="1"/>
+    <col min="9" max="9" width="22.1388888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:13">
+    <row r="1" ht="15.6" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" ht="15.6" spans="1:9">
+      <c r="A2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:13">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="3">
-        <v>2019</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2017</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="WH/Mt. Boucherie Winery"/>
+    <hyperlink ref="H2" r:id="rId1" display="WH/Mt. Boucherie Winery"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1940,34 +1920,34 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="15.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
-    <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
-    <col min="8" max="8" width="20.2857142857143" customWidth="1"/>
-    <col min="9" max="9" width="19.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="10.5740740740741" customWidth="1"/>
+    <col min="3" max="3" width="15.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="10.5740740740741" customWidth="1"/>
+    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="10.8611111111111" customWidth="1"/>
+    <col min="7" max="7" width="12.4259259259259" customWidth="1"/>
+    <col min="8" max="8" width="20.287037037037" customWidth="1"/>
+    <col min="9" max="9" width="19.287037037037" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="35.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
+    <col min="11" max="11" width="35.287037037037" customWidth="1"/>
+    <col min="12" max="12" width="19.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:12">
+    <row r="1" ht="15.6" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -1976,36 +1956,36 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.75" spans="1:12">
+    <row r="2" s="1" customFormat="1" ht="15.6" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3">
         <v>2019</v>
@@ -2026,13 +2006,13 @@
         <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add receipts and returns transfer
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
+    <workbookView windowHeight="17850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
     <sheet name="test_add_Rust" sheetId="4" r:id="rId2"/>
     <sheet name="test_internal_transfer" sheetId="5" r:id="rId3"/>
-    <sheet name="test_transfer_delivery_order" sheetId="6" r:id="rId4"/>
+    <sheet name="test_delivery_order_transfer" sheetId="6" r:id="rId4"/>
+    <sheet name="test_receipts_transfer" sheetId="7" r:id="rId5"/>
+    <sheet name="test_return_transfer" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="78">
   <si>
     <t>Description</t>
   </si>
@@ -228,6 +230,30 @@
   </si>
   <si>
     <t>Sonny International: Delivery Orders</t>
+  </si>
+  <si>
+    <t>Receive_from</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Receipts Transfer" for  MtB product</t>
+  </si>
+  <si>
+    <t>Craig McCulloch</t>
+  </si>
+  <si>
+    <t>Sonny International: Receipts</t>
+  </si>
+  <si>
+    <t>Ware_house</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Return Transfer" for  MtB product</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Sonny International</t>
   </si>
 </sst>
 </file>
@@ -235,10 +261,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -278,6 +304,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -286,18 +349,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,10 +380,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,42 +396,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -370,27 +411,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -399,6 +419,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -407,14 +441,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -431,19 +457,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,163 +559,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,17 +666,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,7 +711,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,16 +735,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -729,11 +757,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -742,148 +768,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -891,13 +917,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1247,78 +1273,78 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="42.1388888888889" customWidth="1"/>
-    <col min="2" max="2" width="22.4444444444444" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.4259259259259" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.4444444444444" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7777777777778" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5740740740741" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1111111111111" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.287037037037" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="22.447619047619" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.4285714285714" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.447619047619" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.7809523809524" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.5714285714286" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.1142857142857" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.6666666666667" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.2857142857143" style="3" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="16.8888888888889" customWidth="1"/>
+    <col min="13" max="13" width="16.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:21">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.75" spans="1:21">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="5" t="s">
@@ -1328,62 +1354,62 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:21">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.75" spans="1:21">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>78235</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="M2" s="6">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T2" s="10" t="s">
@@ -1393,41 +1419,41 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:21">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="15.75" spans="1:21">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>61419</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>2019</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2020</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="M3" s="6">
@@ -1436,19 +1462,19 @@
       <c r="N3" s="6">
         <v>188</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T3" s="10" t="s">
@@ -1458,62 +1484,62 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" ht="16.35" spans="1:21">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="16.5" spans="1:21">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>61419</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2019</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2020</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="6">
         <v>147</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="O4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T4" s="10" t="s">
@@ -1523,62 +1549,62 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" ht="15.6" spans="1:21">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15.75" spans="1:21">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>160920</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2">
         <v>500</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T5" s="11" t="s">
@@ -1603,83 +1629,83 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="41.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="41.447619047619" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.4444444444444" customWidth="1"/>
-    <col min="4" max="4" width="27.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="12.1388888888889" customWidth="1"/>
-    <col min="6" max="6" width="9.42592592592593" customWidth="1"/>
-    <col min="7" max="7" width="9.71296296296296" customWidth="1"/>
-    <col min="8" max="8" width="9.57407407407407" customWidth="1"/>
+    <col min="3" max="3" width="22.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="27.1142857142857" customWidth="1"/>
+    <col min="5" max="5" width="12.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="9.42857142857143" customWidth="1"/>
+    <col min="7" max="7" width="9.71428571428571" customWidth="1"/>
+    <col min="8" max="8" width="9.57142857142857" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.287037037037" customWidth="1"/>
-    <col min="11" max="11" width="9.71296296296296" customWidth="1"/>
-    <col min="12" max="12" width="9.57407407407407" customWidth="1"/>
-    <col min="13" max="13" width="11.8611111111111" customWidth="1"/>
-    <col min="14" max="14" width="11.1388888888889" customWidth="1"/>
-    <col min="15" max="15" width="10.8611111111111" customWidth="1"/>
-    <col min="16" max="16" width="11.287037037037" customWidth="1"/>
-    <col min="19" max="19" width="11.287037037037" customWidth="1"/>
+    <col min="10" max="10" width="10.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="9.71428571428571" customWidth="1"/>
+    <col min="12" max="12" width="9.57142857142857" customWidth="1"/>
+    <col min="13" max="13" width="11.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="11.1428571428571" customWidth="1"/>
+    <col min="15" max="15" width="10.8571428571429" customWidth="1"/>
+    <col min="16" max="16" width="11.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="11.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:21">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.75" spans="1:21">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="5" t="s">
@@ -1689,62 +1715,62 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:21">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.75" spans="1:21">
+      <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>150461</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>2019</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2022</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>2018</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>2021</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>2013</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>1000</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>2000</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>300</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>10</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>246</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>50</v>
       </c>
       <c r="T2" s="13" t="s">
@@ -1754,62 +1780,62 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:21">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="15.75" spans="1:21">
+      <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>150461</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>2020</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2021</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="3">
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>246</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T3" s="13" t="s">
@@ -1830,78 +1856,78 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="29.4444444444444" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5740740740741" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.287037037037" customWidth="1"/>
-    <col min="5" max="5" width="16.8611111111111" customWidth="1"/>
-    <col min="6" max="6" width="10.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="18.4259259259259" customWidth="1"/>
-    <col min="8" max="8" width="19.712962962963" customWidth="1"/>
-    <col min="9" max="9" width="22.1388888888889" customWidth="1"/>
+    <col min="1" max="1" width="37.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="29.447619047619" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5714285714286" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="10.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="18.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="19.7142857142857" customWidth="1"/>
+    <col min="9" max="9" width="22.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.75" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:9">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.75" spans="1:9">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1920,99 +1946,258 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="15.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="20.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="19.2857142857143" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="35.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" s="3" customFormat="1" ht="15.75" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="22.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="16.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="9.42857142857143" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="28.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="10.5740740740741" customWidth="1"/>
-    <col min="3" max="3" width="15.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="10.5740740740741" customWidth="1"/>
-    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="10.8611111111111" customWidth="1"/>
-    <col min="7" max="7" width="12.4259259259259" customWidth="1"/>
-    <col min="8" max="8" width="20.287037037037" customWidth="1"/>
-    <col min="9" max="9" width="19.287037037037" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="35.287037037037" customWidth="1"/>
-    <col min="12" max="12" width="19.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="16.5714285714286" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:12">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.75" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>65</v>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.6" spans="1:12">
-      <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" ht="15.75" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>67</v>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D2" s="3">
-        <v>2019</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2017</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add codes for making orders
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="5" activeTab="10"/>
+    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="test_harvest" sheetId="12" r:id="rId9"/>
     <sheet name="test_add_warehouse_location" sheetId="11" r:id="rId10"/>
     <sheet name="test_search_product" sheetId="13" r:id="rId11"/>
+    <sheet name="test_make_orders" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="134">
   <si>
     <t>Description</t>
   </si>
@@ -367,6 +368,66 @@
   </si>
   <si>
     <t>Bulk Wine</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit_of_Measure</t>
+  </si>
+  <si>
+    <t>Component_location</t>
+  </si>
+  <si>
+    <t>Finished_products_location</t>
+  </si>
+  <si>
+    <t>Component1</t>
+  </si>
+  <si>
+    <t>Component2</t>
+  </si>
+  <si>
+    <t>Component3</t>
+  </si>
+  <si>
+    <t>Consume1</t>
+  </si>
+  <si>
+    <t>Consume2</t>
+  </si>
+  <si>
+    <t>Consume3</t>
+  </si>
+  <si>
+    <t>UoM</t>
+  </si>
+  <si>
+    <t>This is testing for making Bulk Wine</t>
+  </si>
+  <si>
+    <t>Bulk Wine (2022, Chardonnay)</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Winery: Production</t>
+  </si>
+  <si>
+    <t>Grapes (Chardonnay)</t>
+  </si>
+  <si>
+    <t>This is testing for making Bottle Wine</t>
+  </si>
+  <si>
+    <t>Chardonnay MtB-OV</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Floor</t>
   </si>
 </sst>
 </file>
@@ -375,8 +436,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
@@ -396,15 +457,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -437,6 +498,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -445,15 +513,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -477,7 +538,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -492,30 +553,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,14 +577,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,6 +593,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,6 +620,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -573,6 +634,24 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -582,7 +661,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,31 +745,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,7 +787,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,43 +799,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,73 +817,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,30 +846,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -824,6 +861,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -835,6 +881,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,163 +948,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1054,23 +1118,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1401,15 +1465,15 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="42.1388888888889" customWidth="1"/>
-    <col min="2" max="2" width="22.4444444444444" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.4259259259259" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.4444444444444" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.7777777777778" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.5740740740741" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.1111111111111" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.6666666666667" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.287037037037" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.4444444444444" style="7" customWidth="1"/>
+    <col min="3" max="3" width="28.4259259259259" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.4444444444444" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.7777777777778" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.5740740740741" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1111111111111" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.6666666666667" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.287037037037" style="7" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="16.8888888888889" customWidth="1"/>
   </cols>
@@ -1472,270 +1536,270 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:21">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>78235</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="8">
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="9">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="12" t="s">
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.6" spans="1:21">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>61419</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>2019</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2020</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="9">
         <v>18</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="9">
         <v>188</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="12" t="s">
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" ht="16.35" spans="1:21">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>61419</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2019</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2020</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="8">
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="9">
         <v>147</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="12" t="s">
+      <c r="O4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="12" t="s">
+      <c r="U4" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" ht="15.6" spans="1:21">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>160920</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2">
         <v>500</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T5" s="13" t="s">
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1773,24 +1837,24 @@
       <c r="C1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D2" t="s">
@@ -1804,7 +1868,7 @@
       </c>
     </row>
     <row r="3" ht="15.6" spans="1:6">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B3" t="s">
@@ -1819,7 +1883,7 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1834,7 +1898,7 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1856,7 +1920,7 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1864,10 +1928,10 @@
       <c r="A2" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>160920</v>
       </c>
       <c r="D2" t="s">
@@ -1881,7 +1945,7 @@
       <c r="B3" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>150461</v>
       </c>
       <c r="D3" t="s">
@@ -1906,7 +1970,7 @@
       <c r="A5" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C5" t="s">
@@ -1914,6 +1978,163 @@
       </c>
       <c r="D5" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="36.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="31.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="14.1111111111111" customWidth="1"/>
+    <col min="4" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="33.6666666666667" customWidth="1"/>
+    <col min="9" max="10" width="14.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.6" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" ht="15.6" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" ht="15.6" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="2">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2010,140 +2231,140 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:21">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>150461</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>2019</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2022</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>2018</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>2021</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>2013</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>1000</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>2000</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>300</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>10</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>246</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>50</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.6" spans="1:21">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>150461</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>2020</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2021</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="3">
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>246</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="15" t="s">
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="16" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2165,8 +2386,8 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="29.4444444444444" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.5740740740741" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.4444444444444" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.5740740740741" style="7" customWidth="1"/>
     <col min="4" max="4" width="15.287037037037" customWidth="1"/>
     <col min="5" max="5" width="16.8611111111111" customWidth="1"/>
     <col min="6" max="6" width="10.5555555555556" customWidth="1"/>
@@ -2205,31 +2426,31 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2305,41 +2526,41 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" s="6" customFormat="1" ht="15.6" spans="1:12">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="7" customFormat="1" ht="15.6" spans="1:12">
+      <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>2019</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>2017</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>1</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2396,28 +2617,28 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2474,31 +2695,31 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2514,7 +2735,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2560,31 +2781,31 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2642,31 +2863,31 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2744,46 +2965,46 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:14">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>16.9</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <v>7.33</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="7">
         <v>0.66</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add component to consume and save
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="9" activeTab="11"/>
+    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -436,9 +436,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -491,23 +491,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -529,9 +538,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,15 +583,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -562,37 +601,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -613,14 +621,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -637,7 +637,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,91 +805,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,79 +817,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,6 +846,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -863,39 +902,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,17 +943,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -966,130 +966,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1992,7 +1992,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>

</xml_diff>

<commit_message>
add waiting for adding product
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="7" activeTab="11"/>
+    <workbookView windowHeight="17850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -97,15 +97,27 @@
     <t>Winery</t>
   </si>
   <si>
+    <t>MtB Winery - Floor</t>
+  </si>
+  <si>
+    <t>Mt. Boucherie - Bubbles</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>812289165109</t>
+  </si>
+  <si>
+    <t>10122891651097</t>
+  </si>
+  <si>
     <t>MtB Winery - Garage Cellar</t>
   </si>
   <si>
     <t>Modest Wines - Gruner</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>812289292694</t>
   </si>
   <si>
@@ -121,24 +133,21 @@
     <t>10812289192690</t>
   </si>
   <si>
-    <t>MtB Winery - Floor</t>
-  </si>
-  <si>
-    <t>Mt. Boucherie - Bubbles</t>
-  </si>
-  <si>
-    <t>812289165109</t>
-  </si>
-  <si>
-    <t>10122891651097</t>
-  </si>
-  <si>
     <t>This is testing for adding Rust product into ERP system</t>
   </si>
   <si>
     <t>Rust Winery</t>
   </si>
   <si>
+    <t xml:space="preserve">Rust - Gamay </t>
+  </si>
+  <si>
+    <t>812289292584</t>
+  </si>
+  <si>
+    <t>10812289292581</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rust - Gasay </t>
   </si>
   <si>
@@ -152,15 +161,6 @@
   </si>
   <si>
     <t>10812279292591</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rust - Gamay </t>
-  </si>
-  <si>
-    <t>812289292584</t>
-  </si>
-  <si>
-    <t>10812289292581</t>
   </si>
   <si>
     <t>Product_code</t>
@@ -439,10 +439,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -489,44 +489,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -540,9 +526,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,7 +558,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -566,36 +567,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -603,14 +574,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,13 +611,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -641,7 +641,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +743,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,97 +803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,61 +815,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,17 +850,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -869,17 +869,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -904,31 +893,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -947,153 +938,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1128,16 +1128,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1463,26 +1463,26 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="42.1388888888889" customWidth="1"/>
-    <col min="2" max="2" width="22.4444444444444" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28.4259259259259" style="7" customWidth="1"/>
-    <col min="4" max="4" width="29.4444444444444" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.7777777777778" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.5740740740741" style="7" customWidth="1"/>
+    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="22.447619047619" style="7" customWidth="1"/>
+    <col min="3" max="3" width="28.4285714285714" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.447619047619" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.7809523809524" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.5714285714286" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.33333333333333" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.1111111111111" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.1142857142857" style="7" customWidth="1"/>
     <col min="9" max="9" width="14.6666666666667" style="7" customWidth="1"/>
-    <col min="10" max="10" width="11.287037037037" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.2857142857143" style="7" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="16.8888888888889" customWidth="1"/>
+    <col min="13" max="13" width="16.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:21">
+    <row r="1" ht="16.5" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:21">
+    <row r="2" ht="15.75" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>24</v>
       </c>
       <c r="E2" s="2">
-        <v>78235</v>
+        <v>160920</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>25</v>
@@ -1584,8 +1584,8 @@
       <c r="L2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="9">
-        <v>11</v>
+      <c r="M2" s="2">
+        <v>500</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>25</v>
@@ -1608,11 +1608,11 @@
       <c r="T2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:21">
+    <row r="3" ht="15.75" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1620,19 +1620,19 @@
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2">
-        <v>61419</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2020</v>
+        <v>78235</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>25</v>
@@ -1650,10 +1650,10 @@
         <v>25</v>
       </c>
       <c r="M3" s="9">
-        <v>18</v>
-      </c>
-      <c r="N3" s="9">
-        <v>188</v>
+        <v>11</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>25</v>
@@ -1670,14 +1670,14 @@
       <c r="S3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="T3" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" ht="16.35" spans="1:21">
+      <c r="U3" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:21">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1685,10 +1685,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
         <v>61419</v>
@@ -1715,10 +1715,10 @@
         <v>25</v>
       </c>
       <c r="M4" s="9">
-        <v>147</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="N4" s="9">
+        <v>188</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>25</v>
@@ -1735,14 +1735,14 @@
       <c r="S4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" ht="15.6" spans="1:21">
+      <c r="T4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1750,19 +1750,19 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="2">
-        <v>160920</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>61419</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2020</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>25</v>
@@ -1779,11 +1779,11 @@
       <c r="L5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="2">
-        <v>500</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>25</v>
+      <c r="M5" s="9">
+        <v>147</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>25</v>
@@ -1800,7 +1800,7 @@
       <c r="S5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="15" t="s">
         <v>33</v>
       </c>
       <c r="U5" s="15" t="s">
@@ -1822,16 +1822,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="14.3333333333333" customWidth="1"/>
-    <col min="2" max="3" width="19.8888888888889" customWidth="1"/>
+    <col min="2" max="3" width="19.8857142857143" customWidth="1"/>
     <col min="4" max="4" width="28.6666666666667" customWidth="1"/>
-    <col min="5" max="5" width="22.1111111111111" customWidth="1"/>
-    <col min="6" max="6" width="16.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="22.1142857142857" customWidth="1"/>
+    <col min="6" max="6" width="16.1142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:6">
+    <row r="1" ht="15.75" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:6">
+    <row r="2" ht="15.75" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:6">
+    <row r="3" ht="15.75" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
@@ -1906,15 +1906,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="54.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="24.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="11.4444444444444" customWidth="1"/>
-    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="54.7809523809524" customWidth="1"/>
+    <col min="2" max="2" width="24.2190476190476" customWidth="1"/>
+    <col min="3" max="3" width="11.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="17.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:4">
+    <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:4">
+    <row r="2" ht="15.75" spans="1:4">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:4">
+    <row r="3" ht="15.75" spans="1:4">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -1995,24 +1995,24 @@
   <sheetPr/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="36.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="31.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="14.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="36.8857142857143" customWidth="1"/>
+    <col min="2" max="2" width="31.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="14.1142857142857" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="20.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="20.8857142857143" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="33.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="19.7777777777778" customWidth="1"/>
-    <col min="10" max="10" width="14.4444444444444" customWidth="1"/>
+    <col min="9" max="9" width="19.7809523809524" customWidth="1"/>
+    <col min="10" max="10" width="14.447619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:14">
+    <row r="1" ht="15.75" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:14">
+    <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>125</v>
       </c>
@@ -2115,12 +2115,12 @@
       <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:14">
+    <row r="1" ht="15.75" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:14">
+    <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
@@ -2219,32 +2219,32 @@
   <sheetPr/>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="41.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="41.447619047619" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.4444444444444" customWidth="1"/>
-    <col min="4" max="4" width="27.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="12.1388888888889" customWidth="1"/>
-    <col min="6" max="6" width="9.42592592592593" customWidth="1"/>
-    <col min="7" max="7" width="9.71296296296296" customWidth="1"/>
-    <col min="8" max="8" width="9.57407407407407" customWidth="1"/>
+    <col min="3" max="3" width="22.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="27.1142857142857" customWidth="1"/>
+    <col min="5" max="5" width="12.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="9.42857142857143" customWidth="1"/>
+    <col min="7" max="7" width="9.71428571428571" customWidth="1"/>
+    <col min="8" max="8" width="9.57142857142857" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.287037037037" customWidth="1"/>
-    <col min="11" max="11" width="9.71296296296296" customWidth="1"/>
-    <col min="12" max="12" width="9.57407407407407" customWidth="1"/>
-    <col min="13" max="13" width="11.8611111111111" customWidth="1"/>
-    <col min="14" max="14" width="11.1388888888889" customWidth="1"/>
-    <col min="15" max="15" width="10.8611111111111" customWidth="1"/>
-    <col min="16" max="16" width="11.287037037037" customWidth="1"/>
-    <col min="19" max="19" width="11.287037037037" customWidth="1"/>
+    <col min="10" max="10" width="10.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="9.71428571428571" customWidth="1"/>
+    <col min="12" max="12" width="9.57142857142857" customWidth="1"/>
+    <col min="13" max="13" width="11.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="11.1428571428571" customWidth="1"/>
+    <col min="15" max="15" width="10.8571428571429" customWidth="1"/>
+    <col min="16" max="16" width="11.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="11.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:21">
+    <row r="2" ht="15.75" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2326,55 +2326,55 @@
         <v>150461</v>
       </c>
       <c r="F2" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G2" s="8" t="s">
+        <v>2020</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>246</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="2">
-        <v>2022</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2018</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2021</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2013</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="U2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="N2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="O2" s="2">
-        <v>300</v>
-      </c>
-      <c r="P2" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2">
-        <v>246</v>
-      </c>
-      <c r="S2" s="2">
-        <v>50</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="15.6" spans="1:21">
+    </row>
+    <row r="3" ht="15.75" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -2385,52 +2385,52 @@
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>150461</v>
       </c>
       <c r="F3" s="2">
-        <v>2020</v>
-      </c>
-      <c r="G3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2022</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J3" s="2">
         <v>2021</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>25</v>
+      <c r="K3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="O3" s="2">
+        <v>300</v>
+      </c>
+      <c r="P3" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
         <v>246</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>25</v>
+      <c r="S3" s="2">
+        <v>50</v>
       </c>
       <c r="T3" s="16" t="s">
         <v>43</v>
@@ -2454,20 +2454,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="29.4444444444444" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.5740740740741" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.287037037037" customWidth="1"/>
-    <col min="5" max="5" width="16.8611111111111" customWidth="1"/>
-    <col min="6" max="6" width="10.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="18.4259259259259" customWidth="1"/>
-    <col min="8" max="8" width="19.712962962963" customWidth="1"/>
-    <col min="9" max="9" width="22.1388888888889" customWidth="1"/>
+    <col min="1" max="1" width="37.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="29.447619047619" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.5714285714286" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="10.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="18.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="19.7142857142857" customWidth="1"/>
+    <col min="9" max="9" width="22.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:9">
+    <row r="1" ht="15.75" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:9">
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
@@ -2543,23 +2543,23 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="10.5740740740741" customWidth="1"/>
-    <col min="3" max="3" width="15.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="10.5740740740741" customWidth="1"/>
-    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="10.8611111111111" customWidth="1"/>
-    <col min="7" max="7" width="12.4259259259259" customWidth="1"/>
-    <col min="8" max="8" width="20.287037037037" customWidth="1"/>
-    <col min="9" max="9" width="19.287037037037" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="15.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="20.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="19.2857142857143" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="35.287037037037" customWidth="1"/>
-    <col min="12" max="12" width="19.712962962963" customWidth="1"/>
+    <col min="11" max="11" width="35.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:12">
+    <row r="1" ht="15.75" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="1" ht="15.6" spans="1:12">
+    <row r="2" s="7" customFormat="1" ht="15.75" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -2650,18 +2650,18 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="22.4259259259259" customWidth="1"/>
+    <col min="1" max="1" width="22.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="16.1388888888889" customWidth="1"/>
-    <col min="5" max="5" width="9.42592592592593" customWidth="1"/>
+    <col min="3" max="3" width="16.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="9.42857142857143" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="28.5740740740741" customWidth="1"/>
+    <col min="8" max="8" width="28.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:8">
+    <row r="1" ht="15.75" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:8">
+    <row r="2" ht="15.75" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -2728,15 +2728,15 @@
       <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="16.5740740740741" customWidth="1"/>
+    <col min="2" max="2" width="16.5714285714286" customWidth="1"/>
     <col min="7" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.5740740740741" customWidth="1"/>
+    <col min="9" max="9" width="17.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:9">
+    <row r="1" ht="15.75" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:9">
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -2809,20 +2809,20 @@
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="23.4259259259259" customWidth="1"/>
-    <col min="2" max="2" width="28.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="19.5740740740741" customWidth="1"/>
-    <col min="5" max="5" width="14.4259259259259" customWidth="1"/>
-    <col min="6" max="6" width="24.5740740740741" customWidth="1"/>
-    <col min="7" max="7" width="13.8611111111111" customWidth="1"/>
-    <col min="8" max="8" width="23.4259259259259" customWidth="1"/>
-    <col min="9" max="9" width="22.5740740740741" customWidth="1"/>
-    <col min="10" max="10" width="24.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="23.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="28.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="19.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="14.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="24.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="13.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="23.4285714285714" customWidth="1"/>
+    <col min="9" max="9" width="22.5714285714286" customWidth="1"/>
+    <col min="10" max="10" width="24.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:9">
+    <row r="1" ht="15.75" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:9">
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
@@ -2895,16 +2895,16 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="6" max="6" width="23.5740740740741" customWidth="1"/>
-    <col min="7" max="7" width="25.712962962963" customWidth="1"/>
-    <col min="8" max="8" width="24.4259259259259" customWidth="1"/>
-    <col min="9" max="9" width="23.712962962963" customWidth="1"/>
-    <col min="10" max="10" width="33.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="23.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
+    <col min="8" max="8" width="24.4285714285714" customWidth="1"/>
+    <col min="9" max="9" width="23.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="33.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:9">
+    <row r="1" ht="15.75" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:9">
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
@@ -2977,21 +2977,21 @@
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="28.7777777777778" customWidth="1"/>
-    <col min="2" max="3" width="19.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="17.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="21.5555555555556" customWidth="1"/>
-    <col min="9" max="9" width="15.8888888888889" customWidth="1"/>
-    <col min="10" max="10" width="23.5740740740741" customWidth="1"/>
-    <col min="11" max="11" width="25.712962962963" customWidth="1"/>
-    <col min="12" max="13" width="24.4259259259259" customWidth="1"/>
-    <col min="14" max="14" width="23.712962962963" customWidth="1"/>
-    <col min="15" max="15" width="33.4259259259259" customWidth="1"/>
+    <col min="1" max="1" width="28.7809523809524" customWidth="1"/>
+    <col min="2" max="3" width="19.552380952381" customWidth="1"/>
+    <col min="4" max="4" width="17.1142857142857" customWidth="1"/>
+    <col min="5" max="5" width="21.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="15.8857142857143" customWidth="1"/>
+    <col min="10" max="10" width="23.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="25.7142857142857" customWidth="1"/>
+    <col min="12" max="13" width="24.4285714285714" customWidth="1"/>
+    <col min="14" max="14" width="23.7142857142857" customWidth="1"/>
+    <col min="15" max="15" width="33.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:14">
+    <row r="1" ht="15.75" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:14">
+    <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
update scripts for make transfer
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" activeTab="1"/>
+    <workbookView windowHeight="17850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="134">
   <si>
     <t>Description</t>
   </si>
@@ -115,7 +115,25 @@
     <t>MtB Winery - Garage Cellar</t>
   </si>
   <si>
-    <t>Modest Wines - Gruner</t>
+    <t>Modest Wines - By Jove 2019</t>
+  </si>
+  <si>
+    <t>812289192693</t>
+  </si>
+  <si>
+    <t>10812289192690</t>
+  </si>
+  <si>
+    <t>Sonny International</t>
+  </si>
+  <si>
+    <t>SI/Stock</t>
+  </si>
+  <si>
+    <t>Rose 750ml</t>
+  </si>
+  <si>
+    <t>Summit Double Magnum 3L</t>
   </si>
   <si>
     <t>812289292694</t>
@@ -124,15 +142,6 @@
     <t>10812288192695</t>
   </si>
   <si>
-    <t>Modest Wines - By Jove 2019</t>
-  </si>
-  <si>
-    <t>812289192693</t>
-  </si>
-  <si>
-    <t>10812289192690</t>
-  </si>
-  <si>
     <t>This is testing for adding Rust product into ERP system</t>
   </si>
   <si>
@@ -187,9 +196,6 @@
     <t>This is testing "Transfer" with "Internal Transfer" for  MtB product</t>
   </si>
   <si>
-    <t>Summit Double Magnum 3L</t>
-  </si>
-  <si>
     <t>140743-19</t>
   </si>
   <si>
@@ -199,76 +205,69 @@
     <t>Sonny International: Internal Transfers</t>
   </si>
   <si>
+    <t>WH/MtB Winery - Garage Cellar</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>Demand1</t>
+  </si>
+  <si>
+    <t>Demand2</t>
+  </si>
+  <si>
+    <t>Unit_of_Measure2</t>
+  </si>
+  <si>
+    <t>Deliver_address</t>
+  </si>
+  <si>
+    <t>Source_Location</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Delivery Orders" for  MtB product</t>
+  </si>
+  <si>
+    <t>CounterSale-MB</t>
+  </si>
+  <si>
+    <t>Sonny International: Delivery Orders</t>
+  </si>
+  <si>
+    <t>Receive_from</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Receipts Transfer" for  MtB product</t>
+  </si>
+  <si>
+    <t>Craig McCulloch</t>
+  </si>
+  <si>
+    <t>Sonny International: Receipts</t>
+  </si>
+  <si>
+    <t>Ware_house</t>
+  </si>
+  <si>
+    <t>This is testing "Transfer" with "Return Transfer" for  MtB product</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>This is testing 'Sample out' for  MtB product</t>
+  </si>
+  <si>
+    <t>SampleOut</t>
+  </si>
+  <si>
     <t>WH/Mt. Boucherie Winery</t>
   </si>
   <si>
-    <t>SI/Stock</t>
-  </si>
-  <si>
-    <t>Product1</t>
-  </si>
-  <si>
-    <t>Product2</t>
-  </si>
-  <si>
-    <t>Demand1</t>
-  </si>
-  <si>
-    <t>Demand2</t>
-  </si>
-  <si>
-    <t>Unit_of_Measure2</t>
-  </si>
-  <si>
-    <t>Deliver_address</t>
-  </si>
-  <si>
-    <t>Source_Location</t>
-  </si>
-  <si>
-    <t>This is testing "Transfer" with "Delivery Orders" for  MtB product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rose 750ml
-</t>
-  </si>
-  <si>
-    <t>Counter Sale - MB</t>
-  </si>
-  <si>
-    <t>Sonny International: Delivery Orders</t>
-  </si>
-  <si>
-    <t>Receive_from</t>
-  </si>
-  <si>
-    <t>This is testing "Transfer" with "Receipts Transfer" for  MtB product</t>
-  </si>
-  <si>
-    <t>Craig McCulloch</t>
-  </si>
-  <si>
-    <t>Sonny International: Receipts</t>
-  </si>
-  <si>
-    <t>Ware_house</t>
-  </si>
-  <si>
-    <t>This is testing "Transfer" with "Return Transfer" for  MtB product</t>
-  </si>
-  <si>
-    <t>Returns</t>
-  </si>
-  <si>
-    <t>Sonny International</t>
-  </si>
-  <si>
-    <t>This is testing 'Sample out' for  MtB product</t>
-  </si>
-  <si>
-    <t>SampleOut</t>
-  </si>
-  <si>
     <t>This is testing 'Sample in' for  MtB product</t>
   </si>
   <si>
@@ -306,9 +305,6 @@
   </si>
   <si>
     <t>Virtual Locations/Production/WG25164-MB</t>
-  </si>
-  <si>
-    <t>WH/MtB Winery - Garage Cellar</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -439,10 +435,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -495,11 +491,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,15 +531,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,24 +575,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,7 +585,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -597,20 +600,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -641,7 +637,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,6 +649,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -665,55 +805,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,103 +817,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,6 +846,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -861,15 +890,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,32 +919,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -941,9 +935,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -955,6 +951,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -964,136 +963,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1463,7 +1459,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1626,13 +1622,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="2">
-        <v>78235</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>61419</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2020</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>25</v>
@@ -1650,10 +1646,10 @@
         <v>25</v>
       </c>
       <c r="M3" s="9">
-        <v>11</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="N3" s="9">
+        <v>188</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>25</v>
@@ -1682,22 +1678,22 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="2">
-        <v>61419</v>
+        <v>577148</v>
       </c>
       <c r="F4" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2020</v>
+        <v>2017</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>25</v>
@@ -1715,10 +1711,10 @@
         <v>25</v>
       </c>
       <c r="M4" s="9">
-        <v>18</v>
-      </c>
-      <c r="N4" s="9">
-        <v>188</v>
+        <v>147</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>25</v>
@@ -1736,10 +1732,10 @@
         <v>25</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:21">
@@ -1747,22 +1743,22 @@
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="E5" s="2">
-        <v>61419</v>
+        <v>140743</v>
       </c>
       <c r="F5" s="2">
-        <v>2019</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2020</v>
+        <v>2016</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>25</v>
@@ -1780,10 +1776,10 @@
         <v>25</v>
       </c>
       <c r="M5" s="9">
-        <v>147</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>25</v>
@@ -1801,10 +1797,10 @@
         <v>25</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1836,59 +1832,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>101</v>
-      </c>
-      <c r="F2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1925,15 +1921,15 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C2" s="2">
         <v>160920</v>
@@ -1944,21 +1940,21 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>109</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
       </c>
       <c r="C3" s="2">
         <v>150461</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>85</v>
@@ -1972,10 +1968,10 @@
     </row>
     <row r="5" ht="24" customHeight="1" spans="1:4">
       <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -2020,69 +2016,69 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="C2" s="2">
         <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>25</v>
@@ -2128,66 +2124,66 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="C2" s="2">
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>25</v>
@@ -2205,7 +2201,7 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2219,8 +2215,8 @@
   <sheetPr/>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -2311,16 +2307,16 @@
     </row>
     <row r="2" ht="15.75" spans="1:21">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2">
         <v>150461</v>
@@ -2368,24 +2364,24 @@
         <v>25</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:21">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2">
         <v>150461</v>
@@ -2394,7 +2390,7 @@
         <v>2019</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2">
         <v>2022</v>
@@ -2409,7 +2405,7 @@
         <v>2013</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M3" s="2">
         <v>1000</v>
@@ -2433,10 +2429,10 @@
         <v>50</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="U3" s="16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2451,7 +2447,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2461,10 +2457,10 @@
     <col min="3" max="3" width="14.5714285714286" style="7" customWidth="1"/>
     <col min="4" max="4" width="15.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="10.552380952381" customWidth="1"/>
-    <col min="7" max="7" width="18.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="18.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="22.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="19.7142857142857" customWidth="1"/>
-    <col min="9" max="9" width="22.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="29.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:9">
@@ -2475,36 +2471,36 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <v>12</v>
@@ -2513,21 +2509,22 @@
         <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="WH/Mt. Boucherie Winery"/>
+    <hyperlink ref="H2" r:id="rId1" display="SI/Stock"/>
+    <hyperlink ref="I2" r:id="rId1" display="WH/MtB Winery - Garage Cellar"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2540,7 +2537,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2564,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -2576,39 +2573,39 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" ht="15.75" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="2">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="E2" s="2">
         <v>2017</v>
@@ -2632,7 +2629,7 @@
         <v>69</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2644,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -2669,22 +2666,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:8">
@@ -2692,10 +2689,10 @@
         <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <v>24</v>
@@ -2710,7 +2707,7 @@
         <v>73</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2724,8 +2721,8 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2744,25 +2741,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:9">
@@ -2770,10 +2767,10 @@
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <v>24</v>
@@ -2788,10 +2785,10 @@
         <v>76</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2830,36 +2827,36 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <v>24</v>
@@ -2871,13 +2868,13 @@
         <v>72</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2912,25 +2909,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:9">
@@ -2938,10 +2935,10 @@
         <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <v>24</v>
@@ -2956,10 +2953,10 @@
         <v>81</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3008,31 +3005,31 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:14">
@@ -3076,7 +3073,7 @@
         <v>92</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update scripts for make orders
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" activeTab="5"/>
+    <workbookView windowHeight="17850" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
   <si>
     <t>Description</t>
   </si>
@@ -403,31 +403,34 @@
     <t>This is testing for making Bulk Wine</t>
   </si>
   <si>
+    <t>Bulk Wine-2022(Chardonnay)</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Winery: Production</t>
+  </si>
+  <si>
+    <t>WH/MtB Winery - Floor</t>
+  </si>
+  <si>
+    <t>Grapes(Chardonnay)</t>
+  </si>
+  <si>
+    <t>Grapes(Semillon)</t>
+  </si>
+  <si>
+    <t>This is testing for making Bottle Wine</t>
+  </si>
+  <si>
+    <t>Chardonnay MtB-OV</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
     <t>Bulk Wine (2022, Chardonnay)</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Winery: Production</t>
-  </si>
-  <si>
-    <t>Grapes(Chardonnay)</t>
-  </si>
-  <si>
-    <t>Grapes(Semillon)</t>
-  </si>
-  <si>
-    <t>This is testing for making Bottle Wine</t>
-  </si>
-  <si>
-    <t>Chardonnay MtB-OV</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>WH/MtB Winery - Floor</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -484,41 +487,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -529,16 +502,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,6 +527,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,8 +579,31 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,27 +624,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -634,6 +637,66 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -643,7 +706,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,25 +748,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,139 +820,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,24 +845,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,6 +875,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -943,153 +937,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1991,8 +1994,8 @@
   <sheetPr/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2002,7 +2005,8 @@
     <col min="3" max="3" width="14.1142857142857" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="20.8857142857143" customWidth="1"/>
-    <col min="6" max="7" width="20" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="34.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="33.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="19.7809523809524" customWidth="1"/>
     <col min="10" max="10" width="14.447619047619" customWidth="1"/>
@@ -2069,16 +2073,16 @@
         <v>127</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>25</v>
@@ -2162,16 +2166,16 @@
     </row>
     <row r="2" ht="15.75" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C2" s="2">
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>127</v>
@@ -2180,10 +2184,10 @@
         <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>25</v>
@@ -2721,7 +2725,7 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update scripts for samplein
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" firstSheet="4" activeTab="11"/>
+    <workbookView windowHeight="17850" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -262,10 +262,10 @@
     <t>This is testing 'Sample out' for  MtB product</t>
   </si>
   <si>
+    <t>140743-16</t>
+  </si>
+  <si>
     <t>SampleOut</t>
-  </si>
-  <si>
-    <t>WH/Mt. Boucherie Winery</t>
   </si>
   <si>
     <t>This is testing 'Sample in' for  MtB product</t>
@@ -487,6 +487,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -502,23 +517,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,26 +540,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -594,6 +595,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -603,22 +611,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -630,6 +623,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -637,6 +637,156 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -646,7 +796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,163 +808,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,6 +905,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -929,17 +940,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -951,7 +951,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -969,130 +969,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1994,8 +1994,8 @@
   <sheetPr/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2806,8 +2806,8 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2860,7 +2860,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D2" s="7">
         <v>24</v>
@@ -2872,13 +2872,13 @@
         <v>72</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2893,15 +2893,17 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
+    <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="6" max="6" width="23.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
     <col min="8" max="8" width="24.4285714285714" customWidth="1"/>
-    <col min="9" max="9" width="23.7142857142857" customWidth="1"/>
+    <col min="9" max="9" width="31.5714285714286" customWidth="1"/>
     <col min="10" max="10" width="33.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2960,7 +2962,7 @@
         <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update scripts for search
</commit_message>
<xml_diff>
--- a/ui-test/data/excel_data/test_data_erp.xlsx
+++ b/ui-test/data/excel_data/test_data_erp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" firstSheet="4" activeTab="6"/>
+    <workbookView windowHeight="17850" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_MtB" sheetId="3" r:id="rId1"/>
@@ -438,10 +438,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -487,9 +487,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,6 +496,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,9 +517,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,7 +548,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,6 +567,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -589,9 +618,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,35 +630,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -637,6 +637,48 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -646,7 +688,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,31 +748,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,31 +796,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,97 +814,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,17 +849,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -924,25 +933,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,145 +954,145 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1825,7 +1825,7 @@
   <cols>
     <col min="1" max="1" width="14.3333333333333" customWidth="1"/>
     <col min="2" max="3" width="19.8857142857143" customWidth="1"/>
-    <col min="4" max="4" width="28.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="31.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="22.1142857142857" customWidth="1"/>
     <col min="6" max="6" width="16.1142857142857" customWidth="1"/>
   </cols>
@@ -1901,8 +1901,8 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -2806,7 +2806,7 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>